<commit_message>
Update: Product Architecture (pinouts) Starting on the pinouts.  Close to done.
</commit_message>
<xml_diff>
--- a/Kiki/Kiln/2 Architecture/Product Architecture Kiln.xlsx
+++ b/Kiki/Kiln/2 Architecture/Product Architecture Kiln.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="896" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Major Signals List" sheetId="1" state="visible" r:id="rId2"/>
@@ -18,18 +18,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="121">
   <si>
     <t>Project</t>
   </si>
   <si>
+    <t>Kiln</t>
+  </si>
+  <si>
     <t>Author</t>
   </si>
   <si>
     <t>Date</t>
   </si>
   <si>
-    <t>Verison</t>
+    <t>Version</t>
   </si>
   <si>
     <t>Name</t>
@@ -56,31 +59,280 @@
     <t>Max length</t>
   </si>
   <si>
-    <t>High current switch</t>
-  </si>
-  <si>
-    <t>Thermocouple Amplifier</t>
-  </si>
-  <si>
-    <t>Temp selector</t>
-  </si>
-  <si>
-    <t>Display</t>
-  </si>
-  <si>
-    <t>5V power</t>
-  </si>
-  <si>
-    <t>110V power</t>
-  </si>
-  <si>
-    <t>COMPONENT NAME</t>
+    <t>Input width</t>
+  </si>
+  <si>
+    <t>Output width</t>
+  </si>
+  <si>
+    <t>Start button</t>
+  </si>
+  <si>
+    <t>Display signal</t>
+  </si>
+  <si>
+    <t>2.2V</t>
+  </si>
+  <si>
+    <t>20mA * 7</t>
+  </si>
+  <si>
+    <t>Power indicator</t>
+  </si>
+  <si>
+    <t>Heating indicator</t>
+  </si>
+  <si>
+    <t>Ready indicator</t>
+  </si>
+  <si>
+    <t>Amplified Thermocouple signal</t>
+  </si>
+  <si>
+    <t>4.0V</t>
+  </si>
+  <si>
+    <t>20mA</t>
+  </si>
+  <si>
+    <t>Switch control signal</t>
+  </si>
+  <si>
+    <t>5v</t>
+  </si>
+  <si>
+    <t>Element power</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Thinking through the major signals, and documenting that there is no problem</t>
+  </si>
+  <si>
+    <t>Connector pinouts and microcontroller pinouts</t>
+  </si>
+  <si>
+    <t>Kiki Jewell</t>
+  </si>
+  <si>
+    <t>First pass</t>
+  </si>
+  <si>
+    <t>4dig7seg display</t>
+  </si>
+  <si>
+    <t>Arduino Uno</t>
   </si>
   <si>
     <t>Pin Number</t>
   </si>
   <si>
     <t>Pin Name</t>
+  </si>
+  <si>
+    <t>Notes:</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>PD0(RXD)</t>
+  </si>
+  <si>
+    <t>Serial receive</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>PD1(TXD)</t>
+  </si>
+  <si>
+    <t>Serial transmit</t>
+  </si>
+  <si>
+    <t>DP</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>PD2(INT0)</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>PD3(INT1)</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>PD4</t>
+  </si>
+  <si>
+    <t>Dig4</t>
+  </si>
+  <si>
+    <t>Anode</t>
+  </si>
+  <si>
+    <t>PD5</t>
+  </si>
+  <si>
+    <t>Colon(com)</t>
+  </si>
+  <si>
+    <t>PD6</t>
+  </si>
+  <si>
+    <t>Colon</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>PD7</t>
+  </si>
+  <si>
+    <t>PB0</t>
+  </si>
+  <si>
+    <t>Dig3</t>
+  </si>
+  <si>
+    <t>PB1</t>
+  </si>
+  <si>
+    <t>Dig2</t>
+  </si>
+  <si>
+    <t>PB2(SS')</t>
+  </si>
+  <si>
+    <t>SDO</t>
+  </si>
+  <si>
+    <t>PB3(MOSI)</t>
+  </si>
+  <si>
+    <t>Master output</t>
+  </si>
+  <si>
+    <t>SDI</t>
+  </si>
+  <si>
+    <t>PB4(MISO)</t>
+  </si>
+  <si>
+    <t>Master input</t>
+  </si>
+  <si>
+    <t>Dig1</t>
+  </si>
+  <si>
+    <t>SCK</t>
+  </si>
+  <si>
+    <t>PB5(SCK)</t>
+  </si>
+  <si>
+    <t>Clock</t>
+  </si>
+  <si>
+    <t>Thermocouple amplifier</t>
+  </si>
+  <si>
+    <t>A0</t>
+  </si>
+  <si>
+    <t>PC0</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>PC1</t>
+  </si>
+  <si>
+    <t>AGND</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>PC2</t>
+  </si>
+  <si>
+    <t>BIAS</t>
+  </si>
+  <si>
+    <t>To the sensor</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>PC3</t>
+  </si>
+  <si>
+    <t>T-</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>PC4(SDA)</t>
+  </si>
+  <si>
+    <t>I2C data</t>
+  </si>
+  <si>
+    <t>T+</t>
+  </si>
+  <si>
+    <t>A5</t>
+  </si>
+  <si>
+    <t>PC5(SCL)</t>
+  </si>
+  <si>
+    <t>I2C clock</t>
+  </si>
+  <si>
+    <t>AVDD</t>
+  </si>
+  <si>
+    <t>DNC</t>
+  </si>
+  <si>
+    <t>DRDY</t>
+  </si>
+  <si>
+    <t>DVDD</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t>Chip Select pin</t>
+  </si>
+  <si>
+    <t>MISO</t>
+  </si>
+  <si>
+    <t>MOSI</t>
+  </si>
+  <si>
+    <t>FAULT</t>
+  </si>
+  <si>
+    <t>DGND</t>
   </si>
   <si>
     <t>Daily Duty Cycle</t>
@@ -141,7 +393,7 @@
     <numFmt numFmtId="166" formatCode="#,##0.00"/>
     <numFmt numFmtId="167" formatCode="0%"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -177,13 +429,32 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFB3B3B3"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF99CCFF"/>
+        <bgColor rgb="FFCCCCFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -220,7 +491,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -243,6 +514,30 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -270,6 +565,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFB3B3B3"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -278,103 +633,172 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.4387755102041"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.6734693877551"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.5"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.33673469387755"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.5"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="14.5"/>
+    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="14.5"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.8520408163265"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.3673469387755"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.8061224489796"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="14.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="C1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>14</v>
+        <v>19</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>15</v>
+        <v>20</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>16</v>
+        <v>21</v>
+      </c>
+      <c r="J11" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>17</v>
+        <v>22</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="I12" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="J13" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -393,13 +817,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="14.5"/>
@@ -409,39 +833,558 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
+      <c r="B1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4"/>
+        <v>3</v>
+      </c>
+      <c r="B3" s="4" t="n">
+        <v>42645</v>
+      </c>
+      <c r="C3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2"/>
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="0" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="E6" s="0" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>20</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" s="6"/>
+      <c r="E17" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" s="6"/>
+      <c r="E18" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="G20" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="G21" s="0" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="D25" s="6"/>
+      <c r="E25" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="D26" s="6"/>
+      <c r="E26" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="G26" s="0" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="D27" s="6"/>
+      <c r="E27" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="G27" s="0" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C29" s="9"/>
+      <c r="D29" s="6"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="C30" s="10"/>
+      <c r="D30" s="6"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="D32" s="6"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D33" s="6"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="D34" s="6"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="D35" s="6"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="C36" s="10"/>
+      <c r="D36" s="6"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -461,8 +1404,8 @@
   </sheetPr>
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -479,227 +1422,227 @@
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="2"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" s="4"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-    </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="8"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="14"/>
       <c r="E5" s="5"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>23</v>
+    <row r="6" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>107</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="1" t="s">
-        <v>24</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="9" t="n">
+        <v>109</v>
+      </c>
+      <c r="B7" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="C7" s="6" t="n">
+      <c r="C7" s="12" t="n">
         <v>0.35</v>
       </c>
-      <c r="D7" s="6" t="n">
+      <c r="D7" s="12" t="n">
         <f aca="false">B7*C7</f>
         <v>0.35</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="9" t="n">
+        <v>110</v>
+      </c>
+      <c r="B8" s="15" t="n">
         <v>0.05</v>
       </c>
-      <c r="C8" s="6" t="n">
+      <c r="C8" s="12" t="n">
         <v>0.35</v>
       </c>
-      <c r="D8" s="6" t="n">
+      <c r="D8" s="12" t="n">
         <f aca="false">B8*C8</f>
         <v>0.0175</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="9" t="n">
+        <v>111</v>
+      </c>
+      <c r="B9" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="C9" s="6" t="n">
+      <c r="C9" s="12" t="n">
         <v>0.35</v>
       </c>
-      <c r="D9" s="6" t="n">
+      <c r="D9" s="12" t="n">
         <f aca="false">B9*C9</f>
         <v>0.35</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="9" t="n">
+        <v>112</v>
+      </c>
+      <c r="B10" s="15" t="n">
         <v>0.1</v>
       </c>
-      <c r="C10" s="6" t="n">
+      <c r="C10" s="12" t="n">
         <v>0.35</v>
       </c>
-      <c r="D10" s="6" t="n">
+      <c r="D10" s="12" t="n">
         <f aca="false">B10*C10</f>
         <v>0.035</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="9" t="n">
+        <v>113</v>
+      </c>
+      <c r="B11" s="15" t="n">
         <v>0.1</v>
       </c>
-      <c r="C11" s="6" t="n">
+      <c r="C11" s="12" t="n">
         <v>0.35</v>
       </c>
-      <c r="D11" s="6" t="n">
+      <c r="D11" s="12" t="n">
         <f aca="false">B11*C11</f>
         <v>0.035</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="9" t="n">
+        <v>114</v>
+      </c>
+      <c r="B12" s="15" t="n">
         <v>0.1</v>
       </c>
-      <c r="C12" s="6" t="n">
+      <c r="C12" s="12" t="n">
         <v>0.35</v>
       </c>
-      <c r="D12" s="6" t="n">
+      <c r="D12" s="12" t="n">
         <f aca="false">B12*C12</f>
         <v>0.035</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" s="9" t="n">
+        <v>115</v>
+      </c>
+      <c r="B13" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="C13" s="6" t="n">
+      <c r="C13" s="12" t="n">
         <v>0.35</v>
       </c>
-      <c r="D13" s="6" t="n">
+      <c r="D13" s="12" t="n">
         <f aca="false">B13*C13</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B14" s="9" t="n">
+        <v>116</v>
+      </c>
+      <c r="B14" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="C14" s="6" t="n">
+      <c r="C14" s="12" t="n">
         <v>0.35</v>
       </c>
-      <c r="D14" s="6" t="n">
+      <c r="D14" s="12" t="n">
         <f aca="false">B14*C14</f>
         <v>0.35</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" s="9" t="n">
+        <v>117</v>
+      </c>
+      <c r="B15" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="C15" s="6" t="n">
+      <c r="C15" s="12" t="n">
         <v>0.35</v>
       </c>
-      <c r="D15" s="6" t="n">
+      <c r="D15" s="12" t="n">
         <f aca="false">B15*C15</f>
         <v>0.35</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16" s="9" t="n">
+        <v>118</v>
+      </c>
+      <c r="B16" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="C16" s="6" t="n">
+      <c r="C16" s="12" t="n">
         <v>0.35</v>
       </c>
-      <c r="D16" s="6" t="n">
+      <c r="D16" s="12" t="n">
         <f aca="false">B16*C16</f>
         <v>0.35</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B17" s="9" t="n">
+        <v>119</v>
+      </c>
+      <c r="B17" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="C17" s="6" t="n">
+      <c r="C17" s="12" t="n">
         <v>0.35</v>
       </c>
-      <c r="D17" s="6" t="n">
+      <c r="D17" s="12" t="n">
         <f aca="false">B17*C17</f>
         <v>0.35</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
+        <v>120</v>
+      </c>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -720,7 +1663,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -737,19 +1680,19 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" s="2"/>
     </row>

</xml_diff>